<commit_message>
Create test for vs code
</commit_message>
<xml_diff>
--- a/Test/UnitTest/srcTest/mapster.xlsx
+++ b/Test/UnitTest/srcTest/mapster.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>dron</t>
   </si>
@@ -29,6 +29,15 @@
   </si>
   <si>
     <t>asdas</t>
+  </si>
+  <si>
+    <t>rrg</t>
+  </si>
+  <si>
+    <t>g4</t>
+  </si>
+  <si>
+    <t>wer</t>
   </si>
 </sst>
 </file>
@@ -126,7 +135,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -161,7 +170,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -370,15 +379,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="A10" sqref="A10:I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -407,24 +416,80 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>44</v>
+      </c>
+      <c r="C2">
+        <v>324</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>25</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4.55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f>A1&amp;A2</f>
+        <v>dron1</v>
+      </c>
+      <c r="B10" t="str">
+        <f>B1&amp;B2</f>
+        <v>header44</v>
+      </c>
+      <c r="C10" t="str">
+        <f>C1&amp;C2</f>
+        <v>sdds324</v>
+      </c>
+      <c r="D10" t="str">
+        <f>D1&amp;D2</f>
+        <v>asdrrg</v>
+      </c>
+      <c r="E10" t="str">
+        <f>E1&amp;E2</f>
+        <v>asdg4</v>
+      </c>
+      <c r="F10" t="str">
+        <f>F1&amp;F2</f>
+        <v>asd</v>
+      </c>
+      <c r="G10" t="str">
+        <f>G1&amp;G2</f>
+        <v>asd25</v>
+      </c>
+      <c r="H10" t="str">
+        <f>H1&amp;H2</f>
+        <v>asd</v>
+      </c>
+      <c r="I10" t="str">
+        <f>I1&amp;I2</f>
+        <v>asdaswer</v>
       </c>
     </row>
   </sheetData>

</xml_diff>